<commit_message>
Added replication dev cluster
</commit_message>
<xml_diff>
--- a/docs/wp-ip-register.xlsx
+++ b/docs/wp-ip-register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\rjt\ansible\Master3July2019\ops-customer-whitespace-couchbase-deployment\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C711B728-1C9C-4B77-9367-B7217D3F5313}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10256C0D-13FF-4830-92C2-123157E49CA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" tabRatio="748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>Subscription</t>
   </si>
@@ -220,6 +220,32 @@
   </si>
   <si>
     <t>wp-demo-uksouth.internal</t>
+  </si>
+  <si>
+    <t>10.41.0.0/23</t>
+  </si>
+  <si>
+    <t>app-sub 10.41.0.0/24
+appgw-sub 10.41.1.0/24</t>
+  </si>
+  <si>
+    <t>wp-dev-repsrc</t>
+  </si>
+  <si>
+    <t>wp-dev-repsrc-uksouth.internal</t>
+  </si>
+  <si>
+    <t>wp-dev-repdst</t>
+  </si>
+  <si>
+    <t>10.42.0.0/23</t>
+  </si>
+  <si>
+    <t>app-sub 10.42.0.0/24
+appgw-sub 10.42.1.0/24</t>
+  </si>
+  <si>
+    <t>wp-dev-repdst-uksouth.internal</t>
   </si>
 </sst>
 </file>
@@ -708,10 +734,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -959,7 +985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -973,7 +999,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -985,6 +1011,40 @@
       </c>
       <c r="D18" s="2" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1064,6 +1124,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4B727FD08A2A54BBB165E0FA9196374" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e39333214859d4f8c42f9f79b5a5a34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c372d8ee4301dec5f9d1c7779482c32e" ns2:_="">
     <xsd:import namespace="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4"/>
@@ -1221,12 +1287,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA0778A-E145-4DDE-9564-CDD701C6F3CE}">
   <ds:schemaRefs>
@@ -1236,6 +1296,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C235008B-BC02-477C-A8D1-70BF025955C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97F1BB9-C08C-4445-8F0C-148F9082FDAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1251,20 +1327,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C235008B-BC02-477C-A8D1-70BF025955C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding mivapi registry + demosgrep
</commit_message>
<xml_diff>
--- a/docs/wp-ip-register.xlsx
+++ b/docs/wp-ip-register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\rjt\ansible\Master3July2019\ops-customer-whitespace-couchbase-deployment\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10256C0D-13FF-4830-92C2-123157E49CA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984A7179-F8E5-43B8-B93E-0C1EF2AB44CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" tabRatio="748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>Subscription</t>
   </si>
@@ -209,9 +209,6 @@
     <t>10.91.0.0/23</t>
   </si>
   <si>
-    <t>wp-demo-prime-infratestuks-vnet</t>
-  </si>
-  <si>
     <t>10.35.0.0/20</t>
   </si>
   <si>
@@ -246,6 +243,22 @@
   </si>
   <si>
     <t>wp-dev-repdst-uksouth.internal</t>
+  </si>
+  <si>
+    <t>wp-demo-prime-vnet</t>
+  </si>
+  <si>
+    <t>wp-demo-sgrep-vnet</t>
+  </si>
+  <si>
+    <t>10.36.0.0/20</t>
+  </si>
+  <si>
+    <t>wp-demo-sgrep-uksouth.internal</t>
+  </si>
+  <si>
+    <t>app-sub 10.36.0.0/24
+appgw-sub 10.36.1.0/24</t>
   </si>
 </sst>
 </file>
@@ -734,10 +747,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -889,30 +903,33 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -920,13 +937,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -934,13 +951,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -948,13 +965,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -962,10 +979,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>45</v>
@@ -976,13 +993,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -990,10 +1007,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
@@ -1001,16 +1018,16 @@
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -1018,16 +1035,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -1035,16 +1049,33 @@
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="F21" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1057,7 +1088,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A57</xm:sqref>
+          <xm:sqref>A3:A58</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1115,21 +1146,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4B727FD08A2A54BBB165E0FA9196374" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e39333214859d4f8c42f9f79b5a5a34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c372d8ee4301dec5f9d1c7779482c32e" ns2:_="">
     <xsd:import namespace="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4"/>
@@ -1287,10 +1303,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA0778A-E145-4DDE-9564-CDD701C6F3CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97F1BB9-C08C-4445-8F0C-148F9082FDAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1312,19 +1353,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97F1BB9-C08C-4445-8F0C-148F9082FDAF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA0778A-E145-4DDE-9564-CDD701C6F3CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ae882933-2568-4bc8-9eb9-7b0bcd7a5db4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>